<commit_message>
release: versión de prueba 0.1.0 del proyecto
</commit_message>
<xml_diff>
--- a/Prevalidador/archivos/Tapa OPS .xlsx
+++ b/Prevalidador/archivos/Tapa OPS .xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indra365-my.sharepoint.com/personal/dacanonm_indracompany_com/Documents/Documentos/GitHub/automatizacion OPS/Prevalidador/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{9740106F-1614-4473-B123-A727AECFF786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50E37B3E-F1A4-4CED-8880-C6D8D0959C92}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{9740106F-1614-4473-B123-A727AECFF786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74433F01-B105-42F1-93C2-43A36501F3E3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAPA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TAPA!$C$7:$O$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TAPA!$D$7:$P$12</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">TAPA!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +45,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{4290F258-20F5-43D0-82F9-9B7EB361A150}">
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{4290F258-20F5-43D0-82F9-9B7EB361A150}">
       <text>
         <r>
           <rPr>
@@ -848,203 +848,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:U12"/>
+  <dimension ref="D1:V12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="2.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
-    <col min="7" max="7" width="4.54296875" customWidth="1"/>
-    <col min="8" max="8" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.81640625" customWidth="1"/>
-    <col min="10" max="10" width="42.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.453125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="110" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="23.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1796875" style="4" customWidth="1"/>
-    <col min="16" max="17" width="14.1796875" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" style="24"/>
-    <col min="20" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="2.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="4.54296875" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.81640625" customWidth="1"/>
+    <col min="11" max="11" width="42.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.453125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="110" customWidth="1"/>
+    <col min="14" max="14" width="19.453125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="23.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" style="4" customWidth="1"/>
+    <col min="17" max="18" width="14.1796875" customWidth="1"/>
+    <col min="19" max="19" width="11.453125" style="24"/>
+    <col min="21" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="4:22" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="R1"/>
+      <c r="K1" s="4"/>
+      <c r="S1"/>
     </row>
-    <row r="2" spans="3:21" x14ac:dyDescent="0.35">
-      <c r="J2" s="4"/>
-      <c r="R2"/>
+    <row r="2" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="K2" s="4"/>
+      <c r="S2"/>
     </row>
-    <row r="3" spans="3:21" ht="26" x14ac:dyDescent="0.6">
-      <c r="C3" s="26" t="s">
+    <row r="3" spans="4:22" ht="26" x14ac:dyDescent="0.6">
+      <c r="D3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
-      <c r="R3"/>
+      <c r="K3" s="26"/>
+      <c r="S3"/>
     </row>
-    <row r="4" spans="3:21" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="27">
+    <row r="4" spans="4:22" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" s="27">
         <f ca="1">TODAY()</f>
         <v>46072</v>
       </c>
-      <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
-      <c r="R4"/>
+      <c r="K4" s="28"/>
+      <c r="S4"/>
     </row>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.35">
-      <c r="J5" s="4"/>
-      <c r="R5"/>
+    <row r="5" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="K5" s="4"/>
+      <c r="S5"/>
     </row>
-    <row r="6" spans="3:21" ht="21" x14ac:dyDescent="0.5">
-      <c r="C6" s="29" t="s">
+    <row r="6" spans="4:22" ht="21" x14ac:dyDescent="0.5">
+      <c r="D6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="30"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32" t="s">
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="5"/>
-      <c r="R6"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="5"/>
+      <c r="S6"/>
     </row>
-    <row r="7" spans="3:21" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="6" t="s">
+    <row r="7" spans="4:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="O7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="25" t="s">
+      <c r="S7" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="25" t="s">
+      <c r="T7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="25" t="s">
+      <c r="U7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="25" t="s">
+      <c r="V7" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="3:21" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C8" s="10" t="s">
+    <row r="8" spans="4:22" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="11" t="str">
-        <f t="shared" ref="D8:D12" si="0">MID(I8,5,4)</f>
+      <c r="E8" s="11" t="str">
+        <f t="shared" ref="E8:E12" si="0">MID(J8,5,4)</f>
         <v>2222</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="11" t="str">
-        <f t="shared" ref="F8:F12" si="1">MID(I8,12,10)</f>
+      <c r="G8" s="11" t="str">
+        <f t="shared" ref="G8:G12" si="1">MID(J8,12,10)</f>
         <v>222222222</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="14">
+      <c r="I8" s="14">
         <v>2</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="J8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="K8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="L8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="M8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="N8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="O8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="21">
+      <c r="P8" s="21">
         <v>0</v>
       </c>
-      <c r="P8"/>
       <c r="Q8"/>
-      <c r="R8" s="22">
-        <v>1</v>
-      </c>
-      <c r="S8" s="23">
+      <c r="R8"/>
+      <c r="S8" s="22">
         <v>1</v>
       </c>
       <c r="T8" s="23">
@@ -1053,202 +1050,205 @@
       <c r="U8" s="23">
         <v>1</v>
       </c>
+      <c r="V8" s="23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="3:21" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C9" s="10" t="s">
+    <row r="9" spans="4:22" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="E9" s="11" t="str">
         <f t="shared" si="0"/>
         <v>2222</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="11" t="str">
+      <c r="G9" s="11" t="str">
         <f t="shared" si="1"/>
         <v>222222222</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="14">
+      <c r="I9" s="14">
         <v>199</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="M9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="N9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="O9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="21">
+      <c r="P9" s="21">
         <v>0</v>
       </c>
-      <c r="P9"/>
       <c r="Q9"/>
-      <c r="R9" s="22"/>
+      <c r="R9"/>
+      <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="3:21" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C10" s="10" t="s">
+    <row r="10" spans="4:22" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11" t="str">
+      <c r="E10" s="11" t="str">
         <f t="shared" si="0"/>
         <v>3333</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="11" t="str">
+      <c r="G10" s="11" t="str">
         <f t="shared" si="1"/>
         <v>333333333</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="14">
+      <c r="I10" s="14">
         <v>75</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="K10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="L10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="M10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="N10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="O10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="21">
+      <c r="P10" s="21">
         <v>0</v>
       </c>
-      <c r="P10"/>
       <c r="Q10"/>
-      <c r="R10" s="22"/>
+      <c r="R10"/>
+      <c r="S10" s="22"/>
     </row>
-    <row r="11" spans="3:21" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C11" s="10" t="s">
+    <row r="11" spans="4:22" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11" t="str">
+      <c r="E11" s="11" t="str">
         <f t="shared" si="0"/>
         <v>4444</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="11" t="str">
+      <c r="G11" s="11" t="str">
         <f t="shared" si="1"/>
         <v>444444444</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="14">
+      <c r="I11" s="14">
         <v>645</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="L11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="M11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="N11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="O11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="21">
+      <c r="P11" s="21">
         <v>0</v>
       </c>
-      <c r="P11"/>
       <c r="Q11"/>
-      <c r="R11" s="22"/>
+      <c r="R11"/>
+      <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="3:21" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C12" s="10" t="s">
+    <row r="12" spans="4:22" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="11" t="str">
+      <c r="E12" s="11" t="str">
         <f t="shared" si="0"/>
         <v>5555</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="11" t="str">
+      <c r="G12" s="11" t="str">
         <f t="shared" si="1"/>
         <v>555555555</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="14">
+      <c r="I12" s="14">
         <v>30</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="J12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="L12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="M12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="N12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="O12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="21">
+      <c r="P12" s="21">
         <v>0</v>
       </c>
-      <c r="P12"/>
       <c r="Q12"/>
-      <c r="R12" s="22"/>
+      <c r="R12"/>
+      <c r="S12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="K6:M6"/>
   </mergeCells>
-  <conditionalFormatting sqref="K1:K6">
+  <conditionalFormatting sqref="L1:L6">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
+  <conditionalFormatting sqref="L7">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>